<commit_message>
linux allure report generation - 6
</commit_message>
<xml_diff>
--- a/InputFolder/APITemplate.xlsx
+++ b/InputFolder/APITemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\eclipse-workspace\QuickTestAPI-V7\InputFolder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\393042\OneDrive - Cognizant\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7860" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KCSPARTA" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="45">
   <si>
     <t>domain</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>/time/leap</t>
-  </si>
-  <si>
-    <t>asdasd</t>
   </si>
   <si>
     <t>https://kcc-oc-saledocuments-api-qa.cloudhub.io</t>
@@ -198,7 +195,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -629,7 +626,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +656,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -679,7 +676,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -701,7 +698,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4">
         <v>500</v>
@@ -713,10 +710,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D7" s="4"/>
     </row>
@@ -725,10 +722,10 @@
         <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -752,10 +749,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -769,9 +766,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000K-C Internal Only</oddFooter>
-  </headerFooter>
   <customProperties>
     <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
   </customProperties>
@@ -814,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -835,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
@@ -881,13 +875,13 @@
         <v>23</v>
       </c>
       <c r="B8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -904,9 +898,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000K-C Internal Only</oddFooter>
-  </headerFooter>
   <customProperties>
     <customPr name="IbpWorksheetKeyString_GUID" r:id="rId3"/>
   </customProperties>
@@ -917,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,8 +1010,8 @@
       <c r="C8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>28</v>
+      <c r="D8" s="13">
+        <v>1230980</v>
       </c>
     </row>
   </sheetData>
@@ -1037,9 +1028,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000K-C Internal Only</oddFooter>
-  </headerFooter>
   <customProperties>
     <customPr name="IbpWorksheetKeyString_GUID" r:id="rId3"/>
   </customProperties>
@@ -1050,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1153,7 +1141,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,10 +1152,10 @@
         <v>20</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1188,9 +1176,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000K-C Internal Only</oddFooter>
-  </headerFooter>
   <customProperties>
     <customPr name="IbpWorksheetKeyString_GUID" r:id="rId4"/>
   </customProperties>

</xml_diff>

<commit_message>
linux allure report generation - 7
</commit_message>
<xml_diff>
--- a/InputFolder/APITemplate.xlsx
+++ b/InputFolder/APITemplate.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>domain</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>https://postman-echo.com</t>
-  </si>
-  <si>
-    <t>24/10/2016</t>
   </si>
   <si>
     <t>/time/leap</t>
@@ -296,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -340,6 +337,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -656,7 +656,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -676,7 +676,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -698,7 +698,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4">
         <v>500</v>
@@ -710,10 +710,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D7" s="4"/>
     </row>
@@ -722,10 +722,10 @@
         <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -749,10 +749,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -808,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -829,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
@@ -875,13 +875,13 @@
         <v>23</v>
       </c>
       <c r="B8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -909,7 +909,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -1007,8 +1007,8 @@
       <c r="B8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>26</v>
+      <c r="C8" s="17">
+        <v>42410</v>
       </c>
       <c r="D8" s="13">
         <v>1230980</v>
@@ -1141,7 +1141,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1152,10 +1152,10 @@
         <v>20</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allure report generation - added code for both linux and windows
</commit_message>
<xml_diff>
--- a/InputFolder/APITemplate.xlsx
+++ b/InputFolder/APITemplate.xlsx
@@ -909,7 +909,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,10 +1008,10 @@
         <v>24</v>
       </c>
       <c r="C8" s="17">
-        <v>42410</v>
+        <v>42412</v>
       </c>
       <c r="D8" s="13">
-        <v>1230980</v>
+        <v>12309809</v>
       </c>
     </row>
   </sheetData>

</xml_diff>